<commit_message>
updated job status in excel sheet
</commit_message>
<xml_diff>
--- a/daily-update-sheet.xlsx
+++ b/daily-update-sheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="21 August 2019" sheetId="1" r:id="rId1"/>
@@ -63,14 +68,14 @@
     <t>table-au</t>
   </si>
   <si>
-    <t>in progress (along with practical)</t>
+    <t>this topic is completed and updated on github</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +112,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +198,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,21 +409,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" customHeight="1">
+    <row r="1" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" customHeight="1">
+    <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -430,37 +445,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -468,7 +483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -482,24 +497,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>